<commit_message>
commit ajustes adicionales algoritmo
</commit_message>
<xml_diff>
--- a/res/otras bases/FUR PRUEBA - 287727.xlsx
+++ b/res/otras bases/FUR PRUEBA - 287727.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SGRU_laravel\res\otras bases\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5484"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5490"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Acción</t>
   </si>
@@ -68,29 +63,35 @@
     <t>01234567</t>
   </si>
   <si>
-    <t>RESETEAR</t>
-  </si>
-  <si>
     <t>Sandra Vidal</t>
   </si>
   <si>
-    <t xml:space="preserve">TIENDAS FRANQUICIAS </t>
-  </si>
-  <si>
-    <t>CISESAC(VS PROVINCIA)</t>
-  </si>
-  <si>
-    <t>ATIS</t>
-  </si>
-  <si>
-    <t>HUARAZ - LUZURIAGA</t>
+    <t>ALLUS CALL INBOUND</t>
+  </si>
+  <si>
+    <t>ALLUS INBOUND</t>
+  </si>
+  <si>
+    <t>ALLUS INBOUND II</t>
+  </si>
+  <si>
+    <t>+ SIMPLE</t>
+  </si>
+  <si>
+    <t>CALL CENTER IN</t>
+  </si>
+  <si>
+    <t>CREAR</t>
+  </si>
+  <si>
+    <t>GESTOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,7 +216,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -250,7 +251,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -427,35 +428,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -487,15 +488,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2">
-        <v>288028</v>
+        <v>287892</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2">
         <v>12345678</v>
@@ -504,28 +505,28 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2">
-        <v>288028</v>
+        <v>287892</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -534,45 +535,45 @@
         <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2">
-        <v>288028</v>
+        <v>287892</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3">
         <v>23456781</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J4" s="4"/>

</xml_diff>